<commit_message>
file naming updated, and cleaned up. Next up is the ECORP_INDEX_# update to get individual families to ID them into same number to save on batchdata costs, that and updating envs
</commit_message>
<xml_diff>
--- a/Ecorp_Template_Complete.xlsx
+++ b/Ecorp_Template_Complete.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34502B6-2939-D340-A3B8-FFC90DE46B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE680754-9C7C-C64D-98D2-B2A67E7ACF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{7706A7A6-5552-1748-8717-E9B7850FDD75}"/>
+    <workbookView xWindow="18040" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{7706A7A6-5552-1748-8717-E9B7850FDD75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -745,7 +745,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BAA96DD-A6DB-644B-8CA4-11EB01B6094C}">
   <dimension ref="A1:CO6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
far past env files consol. Getting to introducing the v300 Dialer is bringing headaches in the Batchdata process that involved going back & adding better logic. Up next: Coining "Data drops" as hey we're losing certain data in the ETL so we need to plug that back in to Batchdata Upload i.e. other Counties besides Maricopa. Then up next: Get dialer introduced & UI quickly after that
</commit_message>
<xml_diff>
--- a/Ecorp_Template_Complete.xlsx
+++ b/Ecorp_Template_Complete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE680754-9C7C-C64D-98D2-B2A67E7ACF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ABE737-B704-6D45-B8D4-AC0D99D27F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18040" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{7706A7A6-5552-1748-8717-E9B7850FDD75}"/>
+    <workbookView xWindow="18100" yWindow="0" windowWidth="17740" windowHeight="22400" xr2:uid="{7706A7A6-5552-1748-8717-E9B7850FDD75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,39 +50,6 @@
     <t>OWNER_TYPE</t>
   </si>
   <si>
-    <t>Search Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Entity Name(s)</t>
-  </si>
-  <si>
-    <t>Entity ID(s)</t>
-  </si>
-  <si>
-    <t>Entity Type</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Formation Date</t>
-  </si>
-  <si>
-    <t>Business Type</t>
-  </si>
-  <si>
-    <t>Domicile State</t>
-  </si>
-  <si>
-    <t>County</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>ECORP_INDEX_#</t>
   </si>
   <si>
@@ -315,13 +282,46 @@
   </si>
   <si>
     <t>ECORP_URL</t>
+  </si>
+  <si>
+    <t>ECORP_COUNTY</t>
+  </si>
+  <si>
+    <t>ECORP_STATE</t>
+  </si>
+  <si>
+    <t>ECORP_BUSINESS_TYPE</t>
+  </si>
+  <si>
+    <t>ECORP_FORMATION_DATE</t>
+  </si>
+  <si>
+    <t>ECORP_STATUS</t>
+  </si>
+  <si>
+    <t>ECORP_ENTITY_TYPE</t>
+  </si>
+  <si>
+    <t>ECORP_ENTITY_ID_S</t>
+  </si>
+  <si>
+    <t>ECORP_NAME_S</t>
+  </si>
+  <si>
+    <t>ECORP_TYPE</t>
+  </si>
+  <si>
+    <t>ECORP_SEARCH_NAME</t>
+  </si>
+  <si>
+    <t>ECORP_COMMENTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -333,14 +333,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,22 +387,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BAA96DD-A6DB-644B-8CA4-11EB01B6094C}">
-  <dimension ref="A1:CO6"/>
+  <dimension ref="A1:CO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,288 +789,285 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:93" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AE1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AK1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AL1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AM1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AN1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AO1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AP1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AR1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AS1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AT1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AU1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AV1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AW1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AX1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AY1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="BA1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="BB1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="BC1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="BD1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="BE1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BF1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="BG1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BH1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BI1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BK1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BL1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BM1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BN1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BO1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BP1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BR1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BS1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BT1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BU1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BV1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BW1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BX1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BY1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="CA1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="CB1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="CC1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="CD1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="CE1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="CF1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="CG1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="CH1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="CI1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CK1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CL1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CM1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CN1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="CG1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO1" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.2">
-      <c r="K6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>